<commit_message>
Semana 14 | Dia 4 | Redaccion de la fase 4 y 5
</commit_message>
<xml_diff>
--- a/2_data_understanding_module/data_understanding_reports/reporte_datos.xlsx
+++ b/2_data_understanding_module/data_understanding_reports/reporte_datos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Archivo</t>
   </si>
@@ -31,61 +31,22 @@
     <t>Total datos NO Nulos</t>
   </si>
   <si>
-    <t>ci0.csv</t>
-  </si>
-  <si>
-    <t>ci_lca0.csv</t>
-  </si>
-  <si>
-    <t>cncoc.csv</t>
-  </si>
-  <si>
-    <t>cncoec0.csv</t>
-  </si>
-  <si>
-    <t>cncpi0.csv</t>
-  </si>
-  <si>
-    <t>oc0.csv</t>
-  </si>
-  <si>
-    <t>occ.csv</t>
-  </si>
-  <si>
-    <t>ocf0.csv</t>
-  </si>
-  <si>
-    <t>ocs.csv</t>
-  </si>
-  <si>
-    <t>oc_cc0.csv</t>
-  </si>
-  <si>
-    <t>oc_cl0.csv</t>
-  </si>
-  <si>
-    <t>oec0.csv</t>
-  </si>
-  <si>
-    <t>oecc.csv</t>
-  </si>
-  <si>
-    <t>oecf0.csv</t>
-  </si>
-  <si>
-    <t>oecs.csv</t>
-  </si>
-  <si>
-    <t>oec_dr0.csv</t>
-  </si>
-  <si>
-    <t>pcci.csv</t>
-  </si>
-  <si>
-    <t>pcoc.csv</t>
-  </si>
-  <si>
-    <t>pcoec.csv</t>
+    <t>ci_dl_provincia_canton.csv</t>
+  </si>
+  <si>
+    <t>oc_dl_area_especialidad.csv</t>
+  </si>
+  <si>
+    <t>oc_dl_familia_sector_perfil.csv</t>
+  </si>
+  <si>
+    <t>oc_dl_provincia_canton.csv</t>
+  </si>
+  <si>
+    <t>oec_dl_familia_sector_perfil.csv</t>
+  </si>
+  <si>
+    <t>oec_dl_provincia_canton.csv</t>
   </si>
 </sst>
 </file>
@@ -443,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -471,16 +432,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>2970</v>
+        <v>1619</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>17820</v>
+        <v>4857</v>
       </c>
       <c r="E2">
-        <v>17820</v>
+        <v>4857</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -488,16 +449,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>7105</v>
+        <v>2905</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D3">
-        <v>42630</v>
+        <v>8715</v>
       </c>
       <c r="E3">
-        <v>42346</v>
+        <v>8715</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -505,16 +466,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>659</v>
+        <v>222</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4">
-        <v>2636</v>
+        <v>888</v>
       </c>
       <c r="E4">
-        <v>2636</v>
+        <v>888</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -522,16 +483,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>209</v>
+        <v>547</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
-        <v>836</v>
+        <v>1641</v>
       </c>
       <c r="E5">
-        <v>836</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -539,16 +500,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>280</v>
+        <v>2300</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>840</v>
+        <v>9200</v>
       </c>
       <c r="E6">
-        <v>840</v>
+        <v>9200</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -556,237 +517,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>542</v>
+        <v>242</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>5420</v>
+        <v>726</v>
       </c>
       <c r="E7">
-        <v>5333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>36</v>
-      </c>
-      <c r="E8">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>178</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>534</v>
-      </c>
-      <c r="E9">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>5217</v>
-      </c>
-      <c r="C11">
-        <v>7</v>
-      </c>
-      <c r="D11">
-        <v>36519</v>
-      </c>
-      <c r="E11">
-        <v>36519</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>100</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>500</v>
-      </c>
-      <c r="E12">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13">
-        <v>221</v>
-      </c>
-      <c r="C13">
-        <v>10</v>
-      </c>
-      <c r="D13">
-        <v>2210</v>
-      </c>
-      <c r="E13">
-        <v>2210</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
-        <v>14</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14">
-        <v>42</v>
-      </c>
-      <c r="E14">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15">
-        <v>100</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>300</v>
-      </c>
-      <c r="E15">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="D16">
-        <v>12</v>
-      </c>
-      <c r="E16">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17">
-        <v>1205</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17">
-        <v>4820</v>
-      </c>
-      <c r="E17">
-        <v>4604</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18">
-        <v>146010</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="D18">
-        <v>730050</v>
-      </c>
-      <c r="E18">
-        <v>730050</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19">
-        <v>251989</v>
-      </c>
-      <c r="C19">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>2015912</v>
-      </c>
-      <c r="E19">
-        <v>1993246</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20">
-        <v>301572</v>
-      </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>2412576</v>
-      </c>
-      <c r="E20">
-        <v>2412576</v>
+        <v>726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>